<commit_message>
More edits, more code-tweaking, more notes on final things to fix...
</commit_message>
<xml_diff>
--- a/Arriaga_table.xlsx
+++ b/Arriaga_table.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Outcome</t>
   </si>
@@ -73,13 +73,16 @@
   </si>
   <si>
     <t>BF10</t>
+  </si>
+  <si>
+    <t>BF01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +91,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -124,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -134,6 +145,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -436,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F6" sqref="F6:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,24 +464,27 @@
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -480,8 +500,12 @@
       <c r="E2" s="3">
         <v>3.9820820000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>1/E2</f>
+        <v>0.25112491405249815</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
@@ -497,8 +521,12 @@
       <c r="E3" s="3">
         <v>2.1912829999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <f t="shared" ref="F3:F15" si="0">1/E3</f>
+        <v>0.4563536521754607</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -514,8 +542,12 @@
       <c r="E4" s="3">
         <v>0.88357529999999995</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>1.1317654533801478</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -531,8 +563,12 @@
       <c r="E5" s="3">
         <v>0.75882400000000005</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1.3178286401062695</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -548,8 +584,12 @@
       <c r="E6" s="3">
         <v>0.55474140000000005</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1.8026417354104092</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -565,8 +605,12 @@
       <c r="E7" s="3">
         <v>0.53450560000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1.8708877886405679</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -582,8 +626,12 @@
       <c r="E8" s="3">
         <v>0.50294729999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>1.9882798853875943</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -599,8 +647,12 @@
       <c r="E9" s="3">
         <v>0.44720890000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>2.2360914552460827</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -616,8 +668,12 @@
       <c r="E10" s="3">
         <v>0.34290369999999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>2.9162706614131024</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -633,8 +689,12 @@
       <c r="E11" s="3">
         <v>0.33315640000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>3.0015932456948144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -650,8 +710,12 @@
       <c r="E12" s="3">
         <v>0.32391760000000003</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>3.0872048940841741</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -667,8 +731,12 @@
       <c r="E13" s="3">
         <v>0.31235459999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>3.2014895890760053</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -684,8 +752,12 @@
       <c r="E14" s="3">
         <v>0.25548939999999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>3.9140567084192148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -700,6 +772,10 @@
       </c>
       <c r="E15" s="3">
         <v>2.4771459999999999E-2</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>40.369037594069951</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tables now use 1-to-BF or BF-to-1 format. - Anderson et al. 2004 pilot test added to Table 1
</commit_message>
<xml_diff>
--- a/Arriaga_table.xlsx
+++ b/Arriaga_table.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Outcome</t>
   </si>
@@ -76,13 +76,98 @@
   </si>
   <si>
     <t>BF01</t>
+  </si>
+  <si>
+    <t>Arriaga et al., 2008</t>
+  </si>
+  <si>
+    <t>Anderson et al., 2004</t>
+  </si>
+  <si>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Enjoyment</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Frustration</t>
+  </si>
+  <si>
+    <t>Violence</t>
+  </si>
+  <si>
+    <t>&lt;.001</t>
+  </si>
+  <si>
+    <t>1.71-to-1</t>
+  </si>
+  <si>
+    <t>2.39-to-1</t>
+  </si>
+  <si>
+    <t>1-to-2.61</t>
+  </si>
+  <si>
+    <t>1.98-to-1</t>
+  </si>
+  <si>
+    <t>818-to-1</t>
+  </si>
+  <si>
+    <t>1-to-3.98</t>
+  </si>
+  <si>
+    <t>1-to-2.19</t>
+  </si>
+  <si>
+    <t>1.13-to-1</t>
+  </si>
+  <si>
+    <t>1.32-to-1</t>
+  </si>
+  <si>
+    <t>1.80-to-1</t>
+  </si>
+  <si>
+    <t>1.87-to-1</t>
+  </si>
+  <si>
+    <t>1.99-to-1</t>
+  </si>
+  <si>
+    <t>2.24-to-1</t>
+  </si>
+  <si>
+    <t>2.92-to-1</t>
+  </si>
+  <si>
+    <t>3.00-to-1</t>
+  </si>
+  <si>
+    <t>3.09-to-1</t>
+  </si>
+  <si>
+    <t>3.20-to-1</t>
+  </si>
+  <si>
+    <t>3.91-to-1</t>
+  </si>
+  <si>
+    <t>40.4-to-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode=".000"/>
+    <numFmt numFmtId="165" formatCode=".00"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,6 +190,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -114,7 +207,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -131,11 +224,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -143,14 +256,59 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,329 +611,486 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F8"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="12"/>
+    <col min="5" max="5" width="9.140625" style="12" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="0" style="12" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="G1" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B3" s="13">
         <v>2.63</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C3" s="14">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D3" s="15">
         <v>0.53</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E3" s="16">
         <v>3.9820820000000001</v>
       </c>
-      <c r="F2">
-        <f>1/E2</f>
+      <c r="F3" s="12">
+        <f>1/E3</f>
         <v>0.25112491405249815</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="G3" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B4" s="13">
         <v>2.27</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C4" s="14">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D4" s="15">
         <v>0.47</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E4" s="16">
         <v>2.1912829999999999</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F15" si="0">1/E3</f>
+      <c r="F4" s="12">
+        <f t="shared" ref="F4:F16" si="0">1/E4</f>
         <v>0.4563536521754607</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="G4" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B5" s="13">
         <v>1.67</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C5" s="14">
         <v>0.11</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D5" s="15">
         <v>0.37</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E5" s="16">
         <v>0.88357529999999995</v>
       </c>
-      <c r="F4">
+      <c r="F5" s="12">
         <f t="shared" si="0"/>
         <v>1.1317654533801478</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="G5" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B6" s="13">
         <v>1.56</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C6" s="14">
         <v>0.13500000000000001</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D6" s="15">
         <v>0.35</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E6" s="16">
         <v>0.75882400000000005</v>
       </c>
-      <c r="F5">
+      <c r="F6" s="12">
         <f t="shared" si="0"/>
         <v>1.3178286401062695</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="G6" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B7" s="13">
         <v>1.32</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C7" s="14">
         <v>0.20100000000000001</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D7" s="15">
         <v>0.3</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E7" s="16">
         <v>0.55474140000000005</v>
       </c>
-      <c r="F6">
+      <c r="F7" s="12">
         <f t="shared" si="0"/>
         <v>1.8026417354104092</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="G7" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B8" s="13">
         <v>1.29</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C8" s="14">
         <v>0.214</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D8" s="15">
         <v>0.28999999999999998</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E8" s="16">
         <v>0.53450560000000003</v>
       </c>
-      <c r="F7">
+      <c r="F8" s="12">
         <f t="shared" si="0"/>
         <v>1.8708877886405679</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="G8" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B9" s="13">
         <v>1.24</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C9" s="14">
         <v>0.22900000000000001</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D9" s="15">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E9" s="16">
         <v>0.50294729999999999</v>
       </c>
-      <c r="F8">
+      <c r="F9" s="12">
         <f t="shared" si="0"/>
         <v>1.9882798853875943</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="G9" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B10" s="13">
         <v>1.1399999999999999</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C10" s="14">
         <v>0.26700000000000002</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D10" s="15">
         <v>0.26</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E10" s="16">
         <v>0.44720890000000002</v>
       </c>
-      <c r="F9">
+      <c r="F10" s="12">
         <f t="shared" si="0"/>
         <v>2.2360914552460827</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="G10" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B11" s="13">
         <v>0.89</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C11" s="14">
         <v>0.38500000000000001</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D11" s="15">
         <v>0.21</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E11" s="16">
         <v>0.34290369999999998</v>
       </c>
-      <c r="F10">
+      <c r="F11" s="12">
         <f t="shared" si="0"/>
         <v>2.9162706614131024</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="G11" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B12" s="13">
         <v>0.86</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C12" s="14">
         <v>0.39800000000000002</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D12" s="15">
         <v>0.2</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E12" s="16">
         <v>0.33315640000000002</v>
       </c>
-      <c r="F11">
+      <c r="F12" s="12">
         <f t="shared" si="0"/>
         <v>3.0015932456948144</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="G12" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B13" s="13">
         <v>0.83</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C13" s="14">
         <v>0.41899999999999998</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D13" s="15">
         <v>0.19</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E13" s="16">
         <v>0.32391760000000003</v>
       </c>
-      <c r="F12">
+      <c r="F13" s="12">
         <f t="shared" si="0"/>
         <v>3.0872048940841741</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="G13" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B14" s="13">
         <v>0.79</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C14" s="14">
         <v>0.437</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D14" s="15">
         <v>0.18</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E14" s="16">
         <v>0.31235459999999998</v>
       </c>
-      <c r="F13">
+      <c r="F14" s="12">
         <f t="shared" si="0"/>
         <v>3.2014895890760053</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="G14" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B15" s="13">
         <v>0.53</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C15" s="14">
         <v>0.60099999999999998</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D15" s="15">
         <v>0.12</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E15" s="16">
         <v>0.25548939999999998</v>
       </c>
-      <c r="F14">
+      <c r="F15" s="12">
         <f t="shared" si="0"/>
         <v>3.9140567084192148</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="G15" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B16" s="13">
         <v>0.48</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C16" s="14">
         <v>0.63400000000000001</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D16" s="15">
         <v>0.11</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E16" s="16">
         <v>2.4771459999999999E-2</v>
       </c>
-      <c r="F15">
+      <c r="F16" s="12">
         <f t="shared" si="0"/>
         <v>40.369037594069951</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="19"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="19"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="13">
+        <v>1</v>
+      </c>
+      <c r="C19" s="14">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="D19" s="19">
+        <v>0.21</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="13">
+        <v>-0.4</v>
+      </c>
+      <c r="C20" s="14">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="D20" s="19">
+        <v>-0.08</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="13">
+        <v>2.35</v>
+      </c>
+      <c r="C21" s="14">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="D21" s="19">
+        <v>0.45</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="13">
+        <v>-0.79</v>
+      </c>
+      <c r="C22" s="14">
+        <v>0.436</v>
+      </c>
+      <c r="D22" s="19">
+        <v>-0.16600000000000001</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="13">
+        <v>5.48</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="19">
+        <v>0.76</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Struggling to format fucking tables/figures
</commit_message>
<xml_diff>
--- a/Arriaga_table.xlsx
+++ b/Arriaga_table.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Outcome</t>
   </si>
@@ -148,17 +148,58 @@
   </si>
   <si>
     <t>Involvement</t>
+  </si>
+  <si>
+    <r>
+      <t>B</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>01</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pilot test results from Arriaga et al. (2008) and Anderson et al. (2004). Pilot data is largely agnostic between the null and alternative, and in fact sometimes indicates equally strong evidence of certain confounds. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> All Bayes factors rounded to two significant digits.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode=".000"/>
     <numFmt numFmtId="165" formatCode=".00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +222,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -190,7 +252,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -227,11 +289,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -292,6 +365,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -382,6 +461,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -416,6 +496,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -591,23 +672,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="4" width="9.140625" style="12"/>
     <col min="5" max="5" width="9.140625" style="12" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="0" style="12" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" style="12" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -626,11 +708,11 @@
       <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="G1" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -640,7 +722,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="11"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -664,7 +746,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -688,7 +770,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -712,7 +794,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -736,7 +818,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -760,7 +842,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -784,7 +866,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -808,7 +890,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -832,7 +914,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>38</v>
       </c>
@@ -856,7 +938,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>39</v>
       </c>
@@ -880,7 +962,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
@@ -904,7 +986,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>41</v>
       </c>
@@ -928,7 +1010,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>42</v>
       </c>
@@ -952,7 +1034,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>43</v>
       </c>
@@ -976,12 +1058,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="17"/>
       <c r="C17" s="18"/>
       <c r="D17" s="19"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>7</v>
       </c>
@@ -989,7 +1071,7 @@
       <c r="C18" s="18"/>
       <c r="D18" s="19"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
@@ -1006,7 +1088,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>8</v>
       </c>
@@ -1023,7 +1105,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>11</v>
       </c>
@@ -1040,7 +1122,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
@@ -1057,7 +1139,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>12</v>
       </c>
@@ -1073,35 +1155,50 @@
       <c r="G23" s="12" t="s">
         <v>32</v>
       </c>
+    </row>
+    <row r="25" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
     </row>
   </sheetData>
   <sortState ref="A2:E15">
     <sortCondition descending="1" ref="E2:E15"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A25:H25"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>